<commit_message>
use only unique dividends
</commit_message>
<xml_diff>
--- a/transaction_import_template_smaller.xlsx
+++ b/transaction_import_template_smaller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coreyvarma/investments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F584EBF3-97FA-3140-B46C-31D16F1D359B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C31EA9F-A22E-ED44-A08A-32B9F2DE370A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="3500" windowWidth="27640" windowHeight="16940" xr2:uid="{A21784B0-9EE2-A340-9B6A-D4A3F808DD68}"/>
   </bookViews>
@@ -87,6 +87,9 @@
     <t>ONEQ</t>
   </si>
   <si>
+    <t>AAPL</t>
+  </si>
+  <si>
     <t>VOO</t>
   </si>
   <si>
@@ -100,9 +103,6 @@
   </si>
   <si>
     <t>CLF</t>
-  </si>
-  <si>
-    <t>SPY</t>
   </si>
   <si>
     <t>2021-02-27</t>
@@ -505,7 +505,7 @@
   <dimension ref="A1:G299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -584,7 +584,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>

</xml_diff>